<commit_message>
Improved some testing procedures
</commit_message>
<xml_diff>
--- a/data/test_data/TestData.xlsx
+++ b/data/test_data/TestData.xlsx
@@ -20,12 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t xml:space="preserve">useless_column_1</t>
   </si>
   <si>
-    <t xml:space="preserve">numbers</t>
+    <t xml:space="preserve">integers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">float_integers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer_floats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">floats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strings</t>
   </si>
   <si>
     <t xml:space="preserve">dates</t>
@@ -34,13 +46,19 @@
     <t xml:space="preserve">useless_column_2</t>
   </si>
   <si>
-    <t xml:space="preserve">01.01.2011</t>
+    <t xml:space="preserve">1.0</t>
   </si>
   <si>
     <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">6.0</t>
+    <t xml:space="preserve">2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.00001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hello</t>
   </si>
   <si>
     <t xml:space="preserve">02.02.2012</t>
@@ -49,7 +67,13 @@
     <t xml:space="preserve">8</t>
   </si>
   <si>
-    <t xml:space="preserve">11.0</t>
+    <t xml:space="preserve">3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.00001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">world</t>
   </si>
   <si>
     <t xml:space="preserve">03.03.2013</t>
@@ -58,7 +82,7 @@
     <t xml:space="preserve">13</t>
   </si>
   <si>
-    <t xml:space="preserve">99</t>
+    <t xml:space="preserve">4</t>
   </si>
 </sst>
 </file>
@@ -177,12 +201,19 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="9" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="30.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="8.67"/>
   </cols>
@@ -191,19 +222,27 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -218,17 +257,17 @@
       <c r="A2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>8</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -243,19 +282,27 @@
       <c r="A3" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -270,19 +317,27 @@
       <c r="A4" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
@@ -295,21 +350,17 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <v>99</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>

</xml_diff>

<commit_message>
Improved names and tests
</commit_message>
<xml_diff>
--- a/data/test_data/TestData.xlsx
+++ b/data/test_data/TestData.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">2.0</t>
   </si>
   <si>
-    <t xml:space="preserve">2.00001</t>
+    <t xml:space="preserve">2.00501</t>
   </si>
   <si>
     <t xml:space="preserve">hello</t>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">3.0</t>
   </si>
   <si>
-    <t xml:space="preserve">3.00001</t>
+    <t xml:space="preserve">3.00401</t>
   </si>
   <si>
     <t xml:space="preserve">world</t>
@@ -201,18 +201,18 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="13.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="9" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="30.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="8.67"/>

</xml_diff>